<commit_message>
BD: les paramètres nombres doivent être > 0
Sauf deux exceptions
</commit_message>
<xml_diff>
--- a/docs/bd/Dictionnaire de données.xlsx
+++ b/docs/bd/Dictionnaire de données.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgTECBDkeYeRGrPXOmt+knPEcV2bQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjQIW8UyR6h4fjXcp1jzlc6KmXesg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="83">
   <si>
     <t>Table</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Contraintes</t>
   </si>
   <si>
+    <t>Calcul</t>
+  </si>
+  <si>
     <t>Produit</t>
   </si>
   <si>
@@ -48,6 +51,15 @@
     <t>NOT NULL</t>
   </si>
   <si>
+    <t>&gt; 0</t>
+  </si>
+  <si>
+    <t>idCategorie</t>
+  </si>
+  <si>
+    <t>Identifiant de la catégorie</t>
+  </si>
+  <si>
     <t>nom</t>
   </si>
   <si>
@@ -90,15 +102,12 @@
     <t>Quantité de produits en stock</t>
   </si>
   <si>
+    <t>&gt;= 0</t>
+  </si>
+  <si>
     <t>Categorie</t>
   </si>
   <si>
-    <t>idCategorie</t>
-  </si>
-  <si>
-    <t>Identifiant de la catégorie</t>
-  </si>
-  <si>
     <t>idCategorieParent</t>
   </si>
   <si>
@@ -144,7 +153,10 @@
     <t>Définit si le client est agriculteur ou non</t>
   </si>
   <si>
-    <t>BOOLEAN</t>
+    <t>NUMBER(1)</t>
+  </si>
+  <si>
+    <t>0 ou 1</t>
   </si>
   <si>
     <t>Commande</t>
@@ -202,6 +214,9 @@
   </si>
   <si>
     <t>Quantité d'un produit sélectionné dans le panier</t>
+  </si>
+  <si>
+    <t>Quantité du produit dans le panier</t>
   </si>
   <si>
     <t>Reglement</t>
@@ -282,12 +297,12 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -308,18 +323,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border/>
     <border>
       <left style="thin">
@@ -332,11 +347,24 @@
         <color rgb="FF000000"/>
       </top>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -346,7 +374,23 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -354,31 +398,36 @@
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -614,575 +663,719 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="8"/>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="8"/>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="8"/>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7"/>
+      <c r="E10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="7"/>
+      <c r="E14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="7"/>
+      <c r="C16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="8"/>
-      <c r="B17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="7"/>
+      <c r="C17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="8"/>
-      <c r="B18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="7"/>
+      <c r="D18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="7"/>
+      <c r="E22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="D23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="E23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="8"/>
+      <c r="B25" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="C25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="E28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="15"/>
+      <c r="B29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="E29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="13"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="13" t="s">
+      <c r="E30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="C33" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="E33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="E34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="22"/>
+      <c r="B35" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="E37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="D39" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="17"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="12"/>
-      <c r="B37" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="E39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="24"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="B41" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="15"/>
+      <c r="B42" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="17"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="12"/>
-      <c r="B38" s="10" t="s">
+      <c r="C42" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="D42" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="E42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="17"/>
+      <c r="B43" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="17"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12"/>
-      <c r="B39" s="10" t="s">
+      <c r="C43" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="D43" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="E43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="17"/>
+      <c r="B44" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="17"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
+      <c r="C44" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1"/>
     <row r="48" ht="15.75" customHeight="1"/>
@@ -2144,6 +2337,12 @@
     <row r="1004" ht="15.75" customHeight="1"/>
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>